<commit_message>
Public Site: basic functionality reached
</commit_message>
<xml_diff>
--- a/PublicSite/PublicSite/PublicSite/Data.xlsx
+++ b/PublicSite/PublicSite/PublicSite/Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="204">
   <si>
     <t>Computer Science</t>
   </si>
@@ -532,6 +532,102 @@
   </si>
   <si>
     <t>6-9</t>
+  </si>
+  <si>
+    <t>datastruct</t>
+  </si>
+  <si>
+    <t>algo</t>
+  </si>
+  <si>
+    <t>sysprog</t>
+  </si>
+  <si>
+    <t>ver</t>
+  </si>
+  <si>
+    <t>build</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>probdec</t>
+  </si>
+  <si>
+    <t>sysdec</t>
+  </si>
+  <si>
+    <t>com</t>
+  </si>
+  <si>
+    <t>orgfile</t>
+  </si>
+  <si>
+    <t>ordxfile</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>err</t>
+  </si>
+  <si>
+    <t>ide</t>
+  </si>
+  <si>
+    <t>api</t>
+  </si>
+  <si>
+    <t>fw</t>
+  </si>
+  <si>
+    <t>req</t>
+  </si>
+  <si>
+    <t>scr</t>
+  </si>
+  <si>
+    <t>db</t>
+  </si>
+  <si>
+    <t>lang</t>
+  </si>
+  <si>
+    <t>plat</t>
+  </si>
+  <si>
+    <t>yrs</t>
+  </si>
+  <si>
+    <t>dom</t>
+  </si>
+  <si>
+    <t>tool</t>
+  </si>
+  <si>
+    <t>langexp</t>
+  </si>
+  <si>
+    <t>cbaseexp</t>
+  </si>
+  <si>
+    <t>upcom</t>
+  </si>
+  <si>
+    <t>platint</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>blog</t>
   </si>
 </sst>
 </file>
@@ -957,7 +1053,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +1095,9 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>172</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1020,7 +1118,9 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1144,9 @@
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>174</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1065,7 +1167,9 @@
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>175</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1086,7 +1190,9 @@
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1107,7 +1213,9 @@
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1128,7 +1236,9 @@
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1149,7 +1259,9 @@
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
@@ -1170,7 +1282,9 @@
       <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
@@ -1194,7 +1308,9 @@
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
@@ -1215,7 +1331,9 @@
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
@@ -1236,7 +1354,9 @@
       <c r="A13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>34</v>
       </c>
@@ -1260,7 +1380,9 @@
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>34</v>
       </c>
@@ -1281,7 +1403,9 @@
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1302,7 +1426,9 @@
       <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1323,7 +1449,9 @@
       <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1344,7 +1472,9 @@
       <c r="A18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="C18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1368,7 +1498,9 @@
       <c r="A19" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="C19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1389,7 +1521,9 @@
       <c r="A20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>34</v>
       </c>
@@ -1410,7 +1544,9 @@
       <c r="A21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="C21" s="1" t="s">
         <v>34</v>
       </c>
@@ -1431,7 +1567,9 @@
       <c r="A22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="C22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1452,7 +1590,9 @@
       <c r="A23" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>113</v>
       </c>
@@ -1473,7 +1613,9 @@
       <c r="A24" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>113</v>
       </c>
@@ -1494,7 +1636,9 @@
       <c r="A25" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="C25" s="1" t="s">
         <v>113</v>
       </c>
@@ -1515,7 +1659,9 @@
       <c r="A26" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="C26" s="1" t="s">
         <v>113</v>
       </c>
@@ -1536,7 +1682,9 @@
       <c r="A27" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="C27" s="1" t="s">
         <v>128</v>
       </c>
@@ -1557,7 +1705,9 @@
       <c r="A28" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="C28" s="1" t="s">
         <v>128</v>
       </c>
@@ -1578,7 +1728,9 @@
       <c r="A29" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>199</v>
+      </c>
       <c r="C29" s="1" t="s">
         <v>128</v>
       </c>
@@ -1599,7 +1751,9 @@
       <c r="A30" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>128</v>
       </c>
@@ -1620,7 +1774,9 @@
       <c r="A31" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>201</v>
+      </c>
       <c r="C31" s="1" t="s">
         <v>128</v>
       </c>
@@ -1641,7 +1797,9 @@
       <c r="A32" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="C32" s="1" t="s">
         <v>128</v>
       </c>
@@ -1662,7 +1820,9 @@
       <c r="A33" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>128</v>
       </c>

</xml_diff>